<commit_message>
TERCERA ACTUALIZACION DEL TFC 14/11/21
</commit_message>
<xml_diff>
--- a/GIT/PLANIFICACION TFC - ALEJANDRO CANO.xlsx
+++ b/GIT/PLANIFICACION TFC - ALEJANDRO CANO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>octubre</t>
   </si>
@@ -99,9 +99,6 @@
     <t>. CREACION O DEFINICION DE USUARIOS (DIBUJAR LAS FUNCIONES)</t>
   </si>
   <si>
-    <t>. FORMULARIO DE REGISTRO</t>
-  </si>
-  <si>
     <t>. CONEXIONES PHP REGISTRO/ACCESO</t>
   </si>
   <si>
@@ -154,13 +151,34 @@
   </si>
   <si>
     <t>*CREAR UN REPOSITORIO Y SUBIRLO A GITHUB</t>
+  </si>
+  <si>
+    <t>COLOR VERDE = TAREAS COMPLETAS</t>
+  </si>
+  <si>
+    <t>. FORMULARIO DE REGISTRO/ACCESO</t>
+  </si>
+  <si>
+    <t>COLOR NARANJAS = TAREA A MEDIAS</t>
+  </si>
+  <si>
+    <t>COLOR ROJO = TAREAS NO HECHAS</t>
+  </si>
+  <si>
+    <t>*COMENZAR EN EL GUION DE TFC</t>
+  </si>
+  <si>
+    <t>24??</t>
+  </si>
+  <si>
+    <t>9??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +269,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,12 +299,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,19 +334,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,6 +347,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -556,9 +587,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,23 +614,49 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,25 +666,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,7 +1011,7 @@
   <dimension ref="A1:AE42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -987,31 +1024,31 @@
   <sheetData>
     <row r="1" spans="1:24" ht="46.5">
       <c r="A1" s="2"/>
-      <c r="B1" s="36">
+      <c r="B1" s="49">
         <v>2021</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="2"/>
@@ -1067,35 +1104,35 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="2"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="35"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="48"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="33" t="s">
+      <c r="R4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="35"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="48"/>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="2"/>
@@ -1167,7 +1204,7 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="2"/>
-      <c r="B6" s="26"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1181,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="43">
+      <c r="J6" s="35">
         <v>1</v>
       </c>
       <c r="K6" s="10">
@@ -1203,7 +1240,7 @@
         <v>7</v>
       </c>
       <c r="Q6" s="5"/>
-      <c r="R6" s="19"/>
+      <c r="R6" s="18"/>
       <c r="S6" s="9"/>
       <c r="T6" s="10">
         <v>1</v>
@@ -1211,7 +1248,7 @@
       <c r="U6" s="10">
         <v>2</v>
       </c>
-      <c r="V6" s="24">
+      <c r="V6" s="22">
         <v>3</v>
       </c>
       <c r="W6" s="10">
@@ -1223,359 +1260,386 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="2"/>
-      <c r="B7" s="12">
+      <c r="B7" s="40">
         <v>4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>5</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>6</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>7</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>8</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>9</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>10</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="15">
+      <c r="J7" s="14">
         <v>8</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="34">
         <v>9</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="31">
         <v>10</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <v>11</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="12">
         <v>12</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <v>13</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="13">
         <v>14</v>
       </c>
       <c r="Q7" s="5"/>
-      <c r="R7" s="41">
+      <c r="R7" s="33">
         <v>6</v>
       </c>
-      <c r="S7" s="42">
+      <c r="S7" s="34">
         <v>7</v>
       </c>
-      <c r="T7" s="42">
+      <c r="T7" s="34">
         <v>8</v>
       </c>
-      <c r="U7" s="38">
-        <v>9</v>
-      </c>
-      <c r="V7" s="13">
+      <c r="U7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" s="12">
         <v>10</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="12">
         <v>11</v>
       </c>
-      <c r="X7" s="14">
+      <c r="X7" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="2"/>
-      <c r="B8" s="41">
+      <c r="B8" s="33">
         <v>11</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="34">
         <v>12</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>13</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>14</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>15</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>16</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>17</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <v>15</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>16</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="30">
         <v>17</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>18</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="12">
         <v>19</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="12">
         <v>20</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="13">
         <v>21</v>
       </c>
       <c r="Q8" s="5"/>
-      <c r="R8" s="15">
+      <c r="R8" s="14">
         <v>13</v>
       </c>
-      <c r="S8" s="25">
+      <c r="S8" s="23">
         <v>14</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="12">
         <v>15</v>
       </c>
-      <c r="U8" s="13">
+      <c r="U8" s="12">
         <v>16</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>17</v>
       </c>
-      <c r="W8" s="13">
+      <c r="W8" s="12">
         <v>18</v>
       </c>
-      <c r="X8" s="14">
+      <c r="X8" s="13">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="2"/>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>18</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>19</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>20</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>21</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>22</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>23</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>24</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <v>22</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="12">
         <v>23</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="12">
+        <v>25</v>
+      </c>
+      <c r="N9" s="12">
+        <v>26</v>
+      </c>
+      <c r="O9" s="12">
+        <v>27</v>
+      </c>
+      <c r="P9" s="13">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="14">
+        <v>20</v>
+      </c>
+      <c r="S9" s="12">
+        <v>21</v>
+      </c>
+      <c r="T9" s="12">
+        <v>22</v>
+      </c>
+      <c r="U9" s="12">
+        <v>23</v>
+      </c>
+      <c r="V9" s="12">
         <v>24</v>
       </c>
-      <c r="M9" s="13">
+      <c r="W9" s="12">
         <v>25</v>
       </c>
-      <c r="N9" s="13">
-        <v>26</v>
-      </c>
-      <c r="O9" s="13">
-        <v>27</v>
-      </c>
-      <c r="P9" s="14">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="15">
-        <v>20</v>
-      </c>
-      <c r="S9" s="13">
-        <v>21</v>
-      </c>
-      <c r="T9" s="13">
-        <v>22</v>
-      </c>
-      <c r="U9" s="13">
-        <v>23</v>
-      </c>
-      <c r="V9" s="13">
-        <v>24</v>
-      </c>
-      <c r="W9" s="13">
-        <v>25</v>
-      </c>
-      <c r="X9" s="14">
+      <c r="X9" s="13">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="2"/>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>25</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>26</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="30">
         <v>27</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>28</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>29</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>30</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>31</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <v>29</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="12">
         <v>30</v>
       </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="5"/>
-      <c r="R10" s="15">
+      <c r="R10" s="14">
         <v>27</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="12">
         <v>28</v>
       </c>
-      <c r="T10" s="13">
+      <c r="T10" s="12">
         <v>29</v>
       </c>
-      <c r="U10" s="13">
+      <c r="U10" s="12">
         <v>30</v>
       </c>
-      <c r="V10" s="13">
+      <c r="V10" s="12">
         <v>31</v>
       </c>
-      <c r="W10" s="20"/>
-      <c r="X10" s="21"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="20"/>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="2"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
       <c r="Q11" s="5"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="18"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="17"/>
     </row>
     <row r="14" spans="1:24" ht="17.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="F14" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+    </row>
+    <row r="15" spans="1:24" ht="15.75">
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="1:24" ht="17.25">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="18" spans="2:31">
-      <c r="B18" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="F16" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="2:31" ht="15.75">
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="2:31" ht="15.75">
+      <c r="B18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="F18" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
     </row>
     <row r="20" spans="2:31" ht="17.25">
-      <c r="B20" s="37" t="s">
-        <v>43</v>
-      </c>
+      <c r="B20" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
     </row>
     <row r="22" spans="2:31" ht="19.5">
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="R22" s="31" t="s">
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="R22" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="Z22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="Z22" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA22" s="27"/>
-      <c r="AB22" s="27"/>
-      <c r="AC22" s="27"/>
-      <c r="AD22" s="27"/>
-      <c r="AE22" s="27"/>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="21"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
+      <c r="AE22" s="21"/>
     </row>
     <row r="23" spans="2:31">
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="Z23" s="23"/>
-      <c r="AA23" s="23"/>
-      <c r="AB23" s="23"/>
-      <c r="AC23" s="23"/>
-      <c r="AD23" s="23"/>
-      <c r="AE23" s="23"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
     </row>
     <row r="24" spans="2:31" ht="19.5">
       <c r="J24" s="28" t="s">
@@ -1583,171 +1647,171 @@
       </c>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="R24" s="28" t="s">
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="R24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="23"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
     </row>
     <row r="25" spans="2:31" ht="19.5">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23" t="s">
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+    </row>
+    <row r="26" spans="2:31" ht="21">
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23" t="s">
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-    </row>
-    <row r="26" spans="2:31" ht="21">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23" t="s">
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+    </row>
+    <row r="27" spans="2:31" ht="19.5">
+      <c r="B27" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-    </row>
-    <row r="27" spans="2:31" ht="19.5">
-      <c r="B27" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="32" t="s">
-        <v>38</v>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="38" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="2:31" ht="19.5">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="27"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23" t="s">
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="25"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
     </row>
     <row r="29" spans="2:31" ht="19.5">
-      <c r="B29" s="27"/>
-      <c r="C29" s="27" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
       <c r="J29" s="28" t="s">
         <v>19</v>
       </c>
       <c r="K29" s="28"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="R29" s="28" t="s">
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="R29" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="S29" s="28"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
     </row>
     <row r="30" spans="2:31">
-      <c r="B30" s="27"/>
-      <c r="C30" s="27" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="21"/>
     </row>
     <row r="31" spans="2:31" ht="19.5">
       <c r="B31" s="28" t="s">
@@ -1757,151 +1821,151 @@
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23" t="s">
+      <c r="G31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
     </row>
     <row r="32" spans="2:31" ht="19.5">
-      <c r="B32" s="23"/>
-      <c r="C32" s="23" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
       <c r="J32" s="28" t="s">
         <v>20</v>
       </c>
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="R32" s="28" t="s">
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="R32" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="S32" s="28"/>
-      <c r="T32" s="28"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
     </row>
     <row r="33" spans="2:23">
-      <c r="B33" s="23"/>
-      <c r="C33" s="23" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="R33" s="23"/>
-      <c r="S33" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="T33" s="23"/>
-      <c r="U33" s="23"/>
-      <c r="V33" s="23"/>
-      <c r="W33" s="23"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="21"/>
     </row>
     <row r="34" spans="2:23" ht="19.5">
-      <c r="B34" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="J34" s="28" t="s">
+      <c r="B34" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="J34" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="R34" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="R34" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="S34" s="28"/>
-      <c r="T34" s="28"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="23"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
     </row>
     <row r="39" spans="2:23">
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="2:23">
+      <c r="B40" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-    </row>
-    <row r="40" spans="2:23">
-      <c r="B40" s="32" t="s">
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+    </row>
+    <row r="41" spans="2:23">
+      <c r="B41" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-    </row>
-    <row r="41" spans="2:23">
-      <c r="B41" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
     </row>
     <row r="42" spans="2:23">
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>